<commit_message>
building lifetime logic and data updated
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Parameter_Building_Lifetime.xlsx
+++ b/projects/test_building/input/Parameter_Building_Lifetime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8477ED-AFD6-7745-A1BD-CC380475B2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C1A1C8-18C6-CF4C-B357-9AC974FD2280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6100" yWindow="2680" windowWidth="22200" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -436,10 +436,10 @@
         <v>5</v>
       </c>
       <c r="F2">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G2">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -459,10 +459,10 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G3">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -482,10 +482,10 @@
         <v>5</v>
       </c>
       <c r="F4">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G4">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G5">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -528,10 +528,10 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G6">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -551,10 +551,10 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G7">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -574,10 +574,10 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -597,10 +597,10 @@
         <v>5</v>
       </c>
       <c r="F9">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G9">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -620,10 +620,10 @@
         <v>5</v>
       </c>
       <c r="F10">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G10">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -643,10 +643,10 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G11">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -666,10 +666,10 @@
         <v>5</v>
       </c>
       <c r="F12">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G12">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -689,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="F13">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G13">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -712,10 +712,10 @@
         <v>5</v>
       </c>
       <c r="F14">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G14">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -735,10 +735,10 @@
         <v>5</v>
       </c>
       <c r="F15">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G15">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -758,10 +758,10 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G16">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -781,10 +781,10 @@
         <v>5</v>
       </c>
       <c r="F17">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G17">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -804,10 +804,10 @@
         <v>5</v>
       </c>
       <c r="F18">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G18">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -827,10 +827,10 @@
         <v>5</v>
       </c>
       <c r="F19">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G19">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -850,10 +850,10 @@
         <v>5</v>
       </c>
       <c r="F20">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G20">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -873,10 +873,10 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G21">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -896,10 +896,10 @@
         <v>5</v>
       </c>
       <c r="F22">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G22">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -919,10 +919,10 @@
         <v>5</v>
       </c>
       <c r="F23">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G23">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -942,10 +942,10 @@
         <v>5</v>
       </c>
       <c r="F24">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G24">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -965,10 +965,10 @@
         <v>5</v>
       </c>
       <c r="F25">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G25">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -988,10 +988,10 @@
         <v>5</v>
       </c>
       <c r="F26">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G26">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1011,10 +1011,10 @@
         <v>5</v>
       </c>
       <c r="F27">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G27">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1034,10 +1034,10 @@
         <v>5</v>
       </c>
       <c r="F28">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G28">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1057,10 +1057,10 @@
         <v>5</v>
       </c>
       <c r="F29">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G29">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1080,10 +1080,10 @@
         <v>5</v>
       </c>
       <c r="F30">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G30">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1103,10 +1103,10 @@
         <v>5</v>
       </c>
       <c r="F31">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G31">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1126,10 +1126,10 @@
         <v>5</v>
       </c>
       <c r="F32">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G32">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1149,10 +1149,10 @@
         <v>5</v>
       </c>
       <c r="F33">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G33">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1172,10 +1172,10 @@
         <v>5</v>
       </c>
       <c r="F34">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G34">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1195,10 +1195,10 @@
         <v>5</v>
       </c>
       <c r="F35">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G35">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1218,10 +1218,10 @@
         <v>5</v>
       </c>
       <c r="F36">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G36">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1241,10 +1241,10 @@
         <v>5</v>
       </c>
       <c r="F37">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G37">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1264,10 +1264,10 @@
         <v>5</v>
       </c>
       <c r="F38">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G38">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1287,10 +1287,10 @@
         <v>5</v>
       </c>
       <c r="F39">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G39">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1310,10 +1310,10 @@
         <v>5</v>
       </c>
       <c r="F40">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G40">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1333,10 +1333,10 @@
         <v>5</v>
       </c>
       <c r="F41">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G41">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1356,10 +1356,10 @@
         <v>5</v>
       </c>
       <c r="F42">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G42">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1379,10 +1379,10 @@
         <v>5</v>
       </c>
       <c r="F43">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G43">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1402,10 +1402,10 @@
         <v>5</v>
       </c>
       <c r="F44">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G44">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1425,10 +1425,10 @@
         <v>5</v>
       </c>
       <c r="F45">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G45">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,10 +1448,10 @@
         <v>5</v>
       </c>
       <c r="F46">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G46">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1471,10 +1471,10 @@
         <v>5</v>
       </c>
       <c r="F47">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G47">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1494,10 +1494,10 @@
         <v>5</v>
       </c>
       <c r="F48">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G48">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>